<commit_message>
DistrictBattery type added, EnergyAssets config by defaultEnergyAssets
*DistrictBattery gridConnection type has been added to the model
*DistrictBattery defaultEnergyAsset has been added to the defaultEnergyAssets excel
*Configuration of EnergyAssets in the model now works with references to defaultEnergyAssets, to make it possible to add different types of assets from the config-excel easily and leanly.
*KPI-visuals agent has been augmented to include DistrictBattery.
*Total electricity import and export tijdreeksen: fixed double counting error for new timestep.
</commit_message>
<xml_diff>
--- a/Base/db_backboneConfig_industriecase.xlsx
+++ b/Base/db_backboneConfig_industriecase.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\HOUJ\Documents\GitHub\HOLON\Base\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49D8B39A-3E07-40C8-9E81-38A1AF11D7FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCB1FCF7-A125-4A6B-93E1-7B5E63C5628B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{C61B0771-0652-4F35-8DF1-D2D550B8F66D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{C61B0771-0652-4F35-8DF1-D2D550B8F66D}"/>
   </bookViews>
   <sheets>
     <sheet name="config" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="90">
   <si>
     <t>id</t>
   </si>
@@ -114,9 +114,6 @@
     <t>PRODUCTION</t>
   </si>
   <si>
-    <t>PHOTOVOLTAIC</t>
-  </si>
-  <si>
     <t>BUILDING</t>
   </si>
   <si>
@@ -295,6 +292,24 @@
   </si>
   <si>
     <t>Grid_MS_congestion_pricing_production</t>
+  </si>
+  <si>
+    <t>b7</t>
+  </si>
+  <si>
+    <t>DISTRICTBATTERY</t>
+  </si>
+  <si>
+    <t>a3</t>
+  </si>
+  <si>
+    <t>STORAGE</t>
+  </si>
+  <si>
+    <t>Solarpanels_1MW</t>
+  </si>
+  <si>
+    <t>District_Battery_500_kWh</t>
   </si>
 </sst>
 </file>
@@ -365,8 +380,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{0FDC8E75-E660-414B-B3E1-5B0A34732FF0}" name="Table1" displayName="Table1" ref="A1:K7" totalsRowShown="0">
-  <autoFilter ref="A1:K7" xr:uid="{0FDC8E75-E660-414B-B3E1-5B0A34732FF0}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{0FDC8E75-E660-414B-B3E1-5B0A34732FF0}" name="Table1" displayName="Table1" ref="A1:K8" totalsRowShown="0">
+  <autoFilter ref="A1:K8" xr:uid="{0FDC8E75-E660-414B-B3E1-5B0A34732FF0}"/>
   <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{C1F26C42-EF09-4FAE-B3E5-DAEA8219B8D2}" name="index"/>
     <tableColumn id="2" xr3:uid="{9B7F7DBE-603C-4CF1-A73C-0BBF726EF99E}" name="agenttype"/>
@@ -776,7 +791,7 @@
         <v>10</v>
       </c>
       <c r="H1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
@@ -784,7 +799,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C2" t="s">
         <v>2</v>
@@ -802,7 +817,7 @@
         <v>1000</v>
       </c>
       <c r="H2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
@@ -810,7 +825,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C3" t="s">
         <v>1</v>
@@ -825,7 +840,7 @@
         <v>500000</v>
       </c>
       <c r="H3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
@@ -833,7 +848,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C4" t="s">
         <v>3</v>
@@ -842,7 +857,7 @@
         <v>5</v>
       </c>
       <c r="E4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G4" s="1">
         <v>300000</v>
@@ -855,10 +870,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F79AE7D-6C5C-4EEF-8F2D-727C87414EF2}">
-  <dimension ref="A1:K7"/>
+  <dimension ref="A1:K8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -891,22 +906,22 @@
         <v>11</v>
       </c>
       <c r="F1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H1" t="s">
+        <v>29</v>
+      </c>
+      <c r="I1" t="s">
         <v>30</v>
-      </c>
-      <c r="I1" t="s">
-        <v>31</v>
       </c>
       <c r="J1" t="s">
         <v>10</v>
       </c>
       <c r="K1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
@@ -914,22 +929,22 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C2" t="s">
         <v>14</v>
       </c>
       <c r="D2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H2" t="s">
         <v>2</v>
@@ -938,7 +953,7 @@
         <v>50</v>
       </c>
       <c r="K2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
@@ -946,22 +961,22 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C3" t="s">
         <v>15</v>
       </c>
       <c r="D3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H3" t="s">
         <v>2</v>
@@ -970,7 +985,7 @@
         <v>50</v>
       </c>
       <c r="K3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
@@ -978,22 +993,22 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C4" t="s">
         <v>16</v>
       </c>
       <c r="D4" t="s">
+        <v>64</v>
+      </c>
+      <c r="E4" t="s">
         <v>65</v>
       </c>
-      <c r="E4" t="s">
-        <v>66</v>
-      </c>
       <c r="F4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H4" t="s">
         <v>1</v>
@@ -1002,7 +1017,7 @@
         <v>1000</v>
       </c>
       <c r="K4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
@@ -1010,22 +1025,22 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C5" t="s">
         <v>17</v>
       </c>
       <c r="D5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E5" t="s">
+        <v>66</v>
+      </c>
+      <c r="F5" t="s">
+        <v>49</v>
+      </c>
+      <c r="G5" t="s">
         <v>67</v>
-      </c>
-      <c r="F5" t="s">
-        <v>50</v>
-      </c>
-      <c r="G5" t="s">
-        <v>68</v>
       </c>
       <c r="H5" t="s">
         <v>2</v>
@@ -1034,7 +1049,7 @@
         <v>1000</v>
       </c>
       <c r="K5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
@@ -1042,22 +1057,22 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C6" t="s">
         <v>18</v>
       </c>
       <c r="D6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H6" t="s">
         <v>2</v>
@@ -1066,7 +1081,7 @@
         <v>400000</v>
       </c>
       <c r="K6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
@@ -1074,22 +1089,22 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C7" t="s">
         <v>19</v>
       </c>
       <c r="D7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H7" t="s">
         <v>2</v>
@@ -1101,7 +1116,39 @@
         <v>400000</v>
       </c>
       <c r="K7" t="s">
-        <v>39</v>
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>57</v>
+      </c>
+      <c r="C8" t="s">
+        <v>84</v>
+      </c>
+      <c r="D8" t="s">
+        <v>85</v>
+      </c>
+      <c r="E8" t="s">
+        <v>49</v>
+      </c>
+      <c r="F8" t="s">
+        <v>49</v>
+      </c>
+      <c r="G8" t="s">
+        <v>49</v>
+      </c>
+      <c r="H8" t="s">
+        <v>2</v>
+      </c>
+      <c r="J8">
+        <v>1000</v>
+      </c>
+      <c r="K8" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -1142,7 +1189,7 @@
         <v>0</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -1150,16 +1197,16 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -1167,16 +1214,16 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D3" t="s">
+        <v>36</v>
+      </c>
+      <c r="E3" s="4" t="s">
         <v>37</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
@@ -1184,16 +1231,16 @@
         <v>2</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
@@ -1201,16 +1248,16 @@
         <v>3</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
@@ -1218,16 +1265,16 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="7" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
@@ -1235,16 +1282,16 @@
         <v>5</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
@@ -1252,16 +1299,16 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
+        <v>41</v>
+      </c>
+      <c r="C8" t="s">
+        <v>48</v>
+      </c>
+      <c r="D8" t="s">
         <v>42</v>
       </c>
-      <c r="C8" t="s">
-        <v>49</v>
-      </c>
-      <c r="D8" t="s">
-        <v>43</v>
-      </c>
       <c r="E8" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
@@ -1269,16 +1316,16 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
+        <v>52</v>
+      </c>
+      <c r="C9" t="s">
         <v>53</v>
       </c>
-      <c r="C9" t="s">
-        <v>54</v>
-      </c>
       <c r="D9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -1292,10 +1339,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB486294-FB31-4C8F-BAEC-47B37B38DF9C}">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -1328,10 +1375,10 @@
         <v>8</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H1" t="s">
         <v>32</v>
-      </c>
-      <c r="H1" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
@@ -1347,18 +1394,13 @@
       <c r="D2" t="s">
         <v>23</v>
       </c>
-      <c r="E2" t="s">
-        <v>24</v>
+      <c r="E2" s="4" t="s">
+        <v>88</v>
       </c>
       <c r="F2" t="s">
         <v>18</v>
       </c>
-      <c r="G2" s="1">
-        <v>1000</v>
-      </c>
-      <c r="H2">
-        <v>0</v>
-      </c>
+      <c r="G2" s="1"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3">
@@ -1373,17 +1415,32 @@
       <c r="D3" t="s">
         <v>23</v>
       </c>
-      <c r="E3" t="s">
-        <v>24</v>
+      <c r="E3" s="4" t="s">
+        <v>88</v>
       </c>
       <c r="F3" t="s">
         <v>18</v>
       </c>
-      <c r="G3" s="1">
-        <v>1000</v>
-      </c>
-      <c r="H3">
-        <v>0</v>
+      <c r="G3" s="1"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" t="s">
+        <v>86</v>
+      </c>
+      <c r="D4" t="s">
+        <v>87</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="F4" t="s">
+        <v>84</v>
       </c>
     </row>
   </sheetData>
@@ -1409,16 +1466,16 @@
         <v>9</v>
       </c>
       <c r="B1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C1" t="s">
         <v>69</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>70</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>71</v>
-      </c>
-      <c r="E1" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -1426,13 +1483,13 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C2" t="s">
         <v>73</v>
       </c>
-      <c r="C2" t="s">
+      <c r="E2" t="s">
         <v>74</v>
-      </c>
-      <c r="E2" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -1440,16 +1497,16 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C3">
         <v>3</v>
       </c>
       <c r="D3" t="s">
+        <v>76</v>
+      </c>
+      <c r="E3" t="s">
         <v>77</v>
-      </c>
-      <c r="E3" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -1457,16 +1514,16 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C4">
         <v>0.5</v>
       </c>
       <c r="D4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -1474,16 +1531,16 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C5">
         <v>0.7</v>
       </c>
       <c r="D5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
@@ -1491,13 +1548,13 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C6" t="b">
         <v>1</v>
       </c>
       <c r="E6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
@@ -1505,13 +1562,13 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C7" t="b">
         <v>0</v>
       </c>
       <c r="E7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixes for merge with MVP-branche
Fixes for merge with MVPcase-branche
</commit_message>
<xml_diff>
--- a/Base/db_backboneConfig_industriecase.xlsx
+++ b/Base/db_backboneConfig_industriecase.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\HOUJ\Documents\GitHub\HOLON\Base\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCB1FCF7-A125-4A6B-93E1-7B5E63C5628B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EBF85F4-67A7-4D89-AB57-85532742FDAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{C61B0771-0652-4F35-8DF1-D2D550B8F66D}"/>
   </bookViews>
@@ -297,9 +297,6 @@
     <t>b7</t>
   </si>
   <si>
-    <t>DISTRICTBATTERY</t>
-  </si>
-  <si>
     <t>a3</t>
   </si>
   <si>
@@ -309,7 +306,10 @@
     <t>Solarpanels_1MW</t>
   </si>
   <si>
-    <t>District_Battery_500_kWh</t>
+    <t>GRIDBATTERY</t>
+  </si>
+  <si>
+    <t>Grid_battery</t>
   </si>
 </sst>
 </file>
@@ -873,7 +873,7 @@
   <dimension ref="A1:K8"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="G39" sqref="G39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -1130,7 +1130,7 @@
         <v>84</v>
       </c>
       <c r="D8" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="E8" t="s">
         <v>49</v>
@@ -1342,14 +1342,14 @@
   <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="17.33203125" customWidth="1"/>
     <col min="4" max="4" width="17" customWidth="1"/>
-    <col min="5" max="5" width="23.33203125" customWidth="1"/>
+    <col min="5" max="5" width="27.33203125" customWidth="1"/>
     <col min="6" max="6" width="17.33203125" customWidth="1"/>
     <col min="7" max="7" width="19.33203125" customWidth="1"/>
     <col min="8" max="8" width="18.6640625" customWidth="1"/>
@@ -1395,7 +1395,7 @@
         <v>23</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F2" t="s">
         <v>18</v>
@@ -1416,7 +1416,7 @@
         <v>23</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F3" t="s">
         <v>18</v>
@@ -1431,10 +1431,10 @@
         <v>20</v>
       </c>
       <c r="C4" t="s">
+        <v>85</v>
+      </c>
+      <c r="D4" t="s">
         <v>86</v>
-      </c>
-      <c r="D4" t="s">
-        <v>87</v>
       </c>
       <c r="E4" s="4" t="s">
         <v>89</v>

</xml_diff>

<commit_message>
Bottom up mobility behavior
- added a basic AL model to generate profiles for trucks
- added new agent type: 'Mobility tracker' to represent mobility behavior without the energy asset and characteristics (those remain in EnergyAsset and J_EAEV)
- turned off manage charging in GC_household for now
- deleted hardcoded charging treshhold and charging speed in f_configure backbone
- Each gridconnection has a collection of vehicle assets and mobility trackers
</commit_message>
<xml_diff>
--- a/Base/db_backboneConfig_industriecase.xlsx
+++ b/Base/db_backboneConfig_industriecase.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\HOUJ\Documents\GitHub\HOLON\Base\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://tuenl-my.sharepoint.com/personal/p_hogeveen_tue_nl/Documents/HOLON/Base/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EBF85F4-67A7-4D89-AB57-85532742FDAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="13_ncr:1_{2EBF85F4-67A7-4D89-AB57-85532742FDAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E95C7077-1318-4D97-A32C-19FFBFCD26F1}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{C61B0771-0652-4F35-8DF1-D2D550B8F66D}"/>
+    <workbookView xWindow="3765" yWindow="3765" windowWidth="24450" windowHeight="11385" activeTab="2" xr2:uid="{C61B0771-0652-4F35-8DF1-D2D550B8F66D}"/>
   </bookViews>
   <sheets>
     <sheet name="config" sheetId="1" r:id="rId1"/>
@@ -766,6 +766,7 @@
   <cols>
     <col min="2" max="2" width="14" customWidth="1"/>
     <col min="4" max="4" width="13.1640625" customWidth="1"/>
+    <col min="7" max="7" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
@@ -872,7 +873,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F79AE7D-6C5C-4EEF-8F2D-727C87414EF2}">
   <dimension ref="A1:K8"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="G39" sqref="G39"/>
     </sheetView>
   </sheetViews>
@@ -1341,7 +1342,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB486294-FB31-4C8F-BAEC-47B37B38DF9C}">
   <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
@@ -1458,7 +1459,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="32.33203125" customWidth="1"/>
+    <col min="2" max="2" width="40.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">

</xml_diff>